<commit_message>
Update XLS to May 2020 objectives
</commit_message>
<xml_diff>
--- a/AZ-900-objectives.xlsx
+++ b/AZ-900-objectives.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\AZ-900 YouTube Series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Desktop\az900\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD42C5B-6CF1-49B5-9D98-D8A4370B7B91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F624B404-C5DF-482E-A4D7-0CBD0227E7C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="570" windowWidth="19650" windowHeight="15150" tabRatio="169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="15" windowWidth="21270" windowHeight="15510" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AZ-900" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Understand cloud concepts</t>
   </si>
@@ -60,57 +60,9 @@
     <t>Describe some of the core products available in Azure</t>
   </si>
   <si>
-    <t>Describe some of the solutions available on Azure</t>
-  </si>
-  <si>
-    <t>Understand Azure management tools</t>
-  </si>
-  <si>
-    <t>Understand security, privacy, compliance, and trust</t>
-  </si>
-  <si>
-    <t>Understand securing network connectivity in Azure</t>
-  </si>
-  <si>
-    <t>choose an appropriate Azure security solution</t>
-  </si>
-  <si>
     <t>Describe core Azure identity services</t>
   </si>
   <si>
-    <t>Describe security tools and features of Azure</t>
-  </si>
-  <si>
-    <t>Describe Azure governance methodologies</t>
-  </si>
-  <si>
-    <t>Understand monitoring and reporting options in Azure</t>
-  </si>
-  <si>
-    <t>Understand privacy, compliance and data protection standards in Azure</t>
-  </si>
-  <si>
-    <t>determine if Azure is compliant for a business need</t>
-  </si>
-  <si>
-    <t>Understand Azure pricing and support</t>
-  </si>
-  <si>
-    <t>Understand Azure subscriptions</t>
-  </si>
-  <si>
-    <t>Understand planning and management of costs</t>
-  </si>
-  <si>
-    <t>Understand the support options available with Azure</t>
-  </si>
-  <si>
-    <t>Describe Azure Service Level Agreements (SLAs)</t>
-  </si>
-  <si>
-    <t>determine SLA for a particular Azure product or service</t>
-  </si>
-  <si>
     <t>Functional Group</t>
   </si>
   <si>
@@ -126,9 +78,6 @@
     <t>Understand terms such as High Availability, Scalability, Elasticity, Agility, Fault Tolerance, and Disaster Recovery</t>
   </si>
   <si>
-    <t>monitor feature updates and product changes</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -141,63 +90,6 @@
     <t>Understand the consumption-based model</t>
   </si>
   <si>
-    <t>Understand Azure tools such as Azure CLI, PowerShell, and the Azure Portal</t>
-  </si>
-  <si>
-    <t>Understand Azure Advisor</t>
-  </si>
-  <si>
-    <t>Understand the difference between authentication and authorization</t>
-  </si>
-  <si>
-    <t>Understand Azure Security center usage scenarios</t>
-  </si>
-  <si>
-    <t>Understand the use cases and benefits of Azure Monitor and Azure Service Health</t>
-  </si>
-  <si>
-    <t>Understand industry compliance terms such as GDPR, ISO and NIST</t>
-  </si>
-  <si>
-    <t>Understand the Microsoft Privacy Statement</t>
-  </si>
-  <si>
-    <t>Understand Azure Government services (US and Germany)</t>
-  </si>
-  <si>
-    <t>Understand options for purchasing Azure products and services</t>
-  </si>
-  <si>
-    <t>Understand options around Azure Free account</t>
-  </si>
-  <si>
-    <t>Understand the factors affecting costs such as resource types, services, locations, ingress and egress traffic</t>
-  </si>
-  <si>
-    <t>Understand Zones for billing purposes</t>
-  </si>
-  <si>
-    <t>Understand the Pricing calculator</t>
-  </si>
-  <si>
-    <t>Understand the Total Cost of Ownership (TCO) calculator</t>
-  </si>
-  <si>
-    <t>Understand best practices for minimizing Azure costs such as performing cost analysis, creating spending limits and quotas, and using tags to identify cost owners; use Azure reservations; use Azure Advisor recommendations</t>
-  </si>
-  <si>
-    <t>Understand support plans that are available such as Dev, Standard, Professional Direct and Premier</t>
-  </si>
-  <si>
-    <t>Understand how to open a support ticket</t>
-  </si>
-  <si>
-    <t>Understand available support channels outside of support plan channels</t>
-  </si>
-  <si>
-    <t>Understand Public and Private Preview features and how to access them + GA</t>
-  </si>
-  <si>
     <t>Describe Regions and availability zones</t>
   </si>
   <si>
@@ -219,79 +111,151 @@
     <t>Describe the Azure Marketplace and its usage scenarios</t>
   </si>
   <si>
-    <t>Describe Internet of Things (IoT) and products that are available for IoT on Azure such as IoT Fundamentals, IoT Hub and IoT Central</t>
-  </si>
-  <si>
-    <t>Describe Big Data and Analytics and products that are available for Big Data and Analytics such as SQL Data Warehouse, HDInsight and Data Lake Analytics</t>
-  </si>
-  <si>
-    <t>Describe Artificial Intelligence (AI) and products that are available for AI such as Azure Machine Learning Service and Studio</t>
-  </si>
-  <si>
-    <t>Describe Serverless computing and Azure products that are available for serverless computing such as Azure Functions, Logic Apps and App grid</t>
-  </si>
-  <si>
-    <t>Describe the benefits and outcomes of using Azure solutions</t>
-  </si>
-  <si>
-    <t>Describe Azure Firewall</t>
-  </si>
-  <si>
-    <t>Describe Azure DDoS Protection</t>
-  </si>
-  <si>
-    <t>Describe Network Security Group (NSG)</t>
-  </si>
-  <si>
-    <t>Describe Azure Active Directory</t>
-  </si>
-  <si>
-    <t>Describe Azure Multi-Factor Authentication</t>
-  </si>
-  <si>
-    <t>Describe Azure Security</t>
-  </si>
-  <si>
-    <t>Describe Key Vault</t>
-  </si>
-  <si>
-    <t>Describe Azure Information Protection (AIP)</t>
-  </si>
-  <si>
-    <t>Describe Azure Advanced Threat Protection (ATP)</t>
-  </si>
-  <si>
-    <t>Describe Azure Policies and Initiatives</t>
-  </si>
-  <si>
-    <t>Describe Role-Based Access Control (RBAC)</t>
-  </si>
-  <si>
-    <t>Describe Locks</t>
-  </si>
-  <si>
-    <t>Describe Azure Advisor security assistance</t>
-  </si>
-  <si>
-    <t>Describe the Trust center</t>
-  </si>
-  <si>
-    <t>Describe the Service Trust Portal and Compliance Manager</t>
-  </si>
-  <si>
-    <t>Describe an Azure subscription along wit uses and options</t>
-  </si>
-  <si>
-    <t>Describe Azure Cost Management</t>
-  </si>
-  <si>
-    <t>Describe the Knowledge Center</t>
-  </si>
-  <si>
-    <t>Describe a Service Level Agreement (SLA)</t>
-  </si>
-  <si>
-    <t>Understand the service lifecycle in Azure</t>
+    <t>May 2020 Content Catch-Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WVD, ACI, AKS, ExpressRoute, Azure DB for MySQL, PostgreSQL, </t>
+  </si>
+  <si>
+    <t>Describe Core Solutions and Management Tools on Azure</t>
+  </si>
+  <si>
+    <t>Describe core solutions available on Azure</t>
+  </si>
+  <si>
+    <t>Describe solutions for software development including Azure DevOps and Azure DevTest Labs</t>
+  </si>
+  <si>
+    <t>Describe the benefits and usage of IoT Hub, IoT Central, and Azure Sphere</t>
+  </si>
+  <si>
+    <t>Describe the benefits and usage of Azure Synapse Analytics, HDInsight, and Azure Databricks</t>
+  </si>
+  <si>
+    <t>Describe the benefits and usage of Azure Machine Learning, Cognitive Services, and Azure Bot Service</t>
+  </si>
+  <si>
+    <t>Describe the benefits and usage of serverless computing solutions that include Azure Functions, Logic Apps, and Event Grid</t>
+  </si>
+  <si>
+    <t>Describe Azure management tools</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of the Azure portal, Azure PowerShell, Azure CLI, Cloud Shell, and Azure Mobile App</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Advisor</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Monitor</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Service Health</t>
+  </si>
+  <si>
+    <t>Describe General Security and Network Security Features</t>
+  </si>
+  <si>
+    <t>Describe Azure security features</t>
+  </si>
+  <si>
+    <t>Describe basic features of Azure Security Center, policy compliance, security alerts, secure score, and resource hygiene</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Key Vault</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Sentinel</t>
+  </si>
+  <si>
+    <t>Describe Azure network security</t>
+  </si>
+  <si>
+    <t>Describe defense in depth</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of NSGs</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Firewall</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of DDoS Protection</t>
+  </si>
+  <si>
+    <t>Describe Identity, Governance, Privacy, and Compliance Features</t>
+  </si>
+  <si>
+    <t>Explain the difference between authentication and authorization</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Active Directory</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Conditional Access and MFA</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of RBAC</t>
+  </si>
+  <si>
+    <t>Describe Azure governance features</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Policy</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of resource locks</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of tags</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Blueprints</t>
+  </si>
+  <si>
+    <t>Describe privacy and compliance resources</t>
+  </si>
+  <si>
+    <t>Describe the purpose of the MS Privacy Statement and the Cloud Adoption Framework</t>
+  </si>
+  <si>
+    <t>Describe the purpose of the Trust Center</t>
+  </si>
+  <si>
+    <t>Describe the purpose of the Service Trust Portal</t>
+  </si>
+  <si>
+    <t>Describe the purpose of Azure Sovereign Regions (Azure Government cloud services and Azure China cloud services)</t>
+  </si>
+  <si>
+    <t>Describe Azure Pricing and Support</t>
+  </si>
+  <si>
+    <t>Describe methods for planning and management of costs</t>
+  </si>
+  <si>
+    <t>Identity the factors affecting costs (resource types, services, locations, ingress/egress traffic, reserved instances, hybrid use benefit)</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of the Pricing Calculator and TCO Calculator</t>
+  </si>
+  <si>
+    <t>Describe the functionality and usage of Azure Cost Management</t>
+  </si>
+  <si>
+    <t>Describe Azure SLAs and service lifecycles</t>
+  </si>
+  <si>
+    <t>Describe the purpose of an Azure SLA</t>
+  </si>
+  <si>
+    <t>Interpret the terms of an SLA</t>
+  </si>
+  <si>
+    <t>Describe the service lifecycle in Azure (public preview and general availability)</t>
+  </si>
+  <si>
+    <t>AZ-900 Exam Strategy</t>
   </si>
 </sst>
 </file>
@@ -307,21 +271,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -330,6 +279,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,16 +331,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,38 +621,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="106.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3">
@@ -703,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -713,7 +677,7 @@
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
@@ -723,7 +687,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -733,7 +697,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -771,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5">
         <v>8</v>
@@ -781,7 +745,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5">
         <v>9</v>
@@ -793,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -803,7 +767,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5">
         <v>11</v>
@@ -813,7 +777,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5">
         <v>12</v>
@@ -823,7 +787,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5">
         <v>13</v>
@@ -833,199 +797,205 @@
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D21" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D25" s="5">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="C26" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D27" s="5">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C29" s="4" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D29" s="5">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D30" s="5">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D31" s="5">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D32" s="5">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="C33" s="4" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D33" s="5">
         <v>32</v>
@@ -1035,7 +1005,7 @@
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D34" s="5">
         <v>33</v>
@@ -1043,11 +1013,9 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D35" s="5">
         <v>34</v>
@@ -1057,7 +1025,7 @@
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D36" s="5">
         <v>35</v>
@@ -1065,9 +1033,11 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D37" s="5">
         <v>36</v>
@@ -1077,31 +1047,27 @@
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D38" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D39" s="5">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D40" s="5">
         <v>39</v>
@@ -1109,9 +1075,11 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C41" s="4" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5">
         <v>40</v>
@@ -1121,7 +1089,7 @@
       <c r="A42" s="2"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D42" s="5">
         <v>41</v>
@@ -1131,41 +1099,41 @@
       <c r="A43" s="2"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D43" s="5">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D44" s="5">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="4"/>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C45" s="4" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D45" s="5">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D46" s="5">
         <v>45</v>
@@ -1173,11 +1141,9 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D47" s="5">
         <v>46</v>
@@ -1185,169 +1151,138 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="C48" s="4" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D48" s="5">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D49" s="5">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D50" s="5">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D51" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C52" s="4"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="5">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="5">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="B55" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="5">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D56" s="5">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="5">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" s="5">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D59" s="5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="5">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="4"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D61" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="4"/>
-      <c r="C62" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="5">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="5">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="5">
-        <v>63</v>
-      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C64" s="4"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="4"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add hyperlinks to XLSX
</commit_message>
<xml_diff>
--- a/AZ-900-objectives.xlsx
+++ b/AZ-900-objectives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Desktop\az900\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Desktop/az900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F624B404-C5DF-482E-A4D7-0CBD0227E7C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C2F56F-2F0C-3744-8DC8-63F52BDE0014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="15" windowWidth="21270" windowHeight="15510" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="47960" windowHeight="24160" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AZ-900" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Understand cloud concepts</t>
   </si>
@@ -256,6 +256,75 @@
   </si>
   <si>
     <t>AZ-900 Exam Strategy</t>
+  </si>
+  <si>
+    <t>Episode Title / Hyperlink</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Cloud Computing Vocabulary</t>
+  </si>
+  <si>
+    <t>Economies of Scale</t>
+  </si>
+  <si>
+    <t>CapEx vs. OpEx</t>
+  </si>
+  <si>
+    <t>Consumption Pricing Model</t>
+  </si>
+  <si>
+    <t>IaaS, PaaS, and SaaS</t>
+  </si>
+  <si>
+    <t>Cloud Deployment Models</t>
+  </si>
+  <si>
+    <t>Regions and Availability Zones</t>
+  </si>
+  <si>
+    <t>Azure Resource Manager</t>
+  </si>
+  <si>
+    <t>Azure Compute Products</t>
+  </si>
+  <si>
+    <t>Azure Networking Products</t>
+  </si>
+  <si>
+    <t>Azure Storage Products</t>
+  </si>
+  <si>
+    <t>Azure Database Products</t>
+  </si>
+  <si>
+    <t>Azure Marketplace</t>
+  </si>
+  <si>
+    <t>Content Catch-Up</t>
+  </si>
+  <si>
+    <t>Azure IoT Products</t>
+  </si>
+  <si>
+    <t>Azure Big Data Analytics Products</t>
+  </si>
+  <si>
+    <t>Azure AI Products</t>
+  </si>
+  <si>
+    <t>Azure Serverless Computing Products</t>
+  </si>
+  <si>
+    <t>Azure Software Dev Products</t>
+  </si>
+  <si>
+    <t>Azure Management Tools</t>
+  </si>
+  <si>
+    <t>Azure Advisor</t>
   </si>
 </sst>
 </file>
@@ -292,8 +361,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -322,10 +392,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,9 +411,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,20 +699,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="2" max="3" width="48.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -646,11 +722,14 @@
       <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -658,8 +737,11 @@
       <c r="D2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,8 +754,11 @@
       <c r="D3" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -682,8 +767,11 @@
       <c r="D4" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -692,8 +780,11 @@
       <c r="D5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -702,8 +793,11 @@
       <c r="D6" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -714,8 +808,11 @@
       <c r="D7" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -726,8 +823,11 @@
       <c r="D8" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -740,8 +840,11 @@
       <c r="D9" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
@@ -750,8 +853,11 @@
       <c r="D10" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>8</v>
@@ -762,8 +868,11 @@
       <c r="D11" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -772,8 +881,11 @@
       <c r="D12" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -782,8 +894,11 @@
       <c r="D13" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -792,8 +907,11 @@
       <c r="D14" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -802,8 +920,11 @@
       <c r="D15" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -814,8 +935,11 @@
       <c r="D16" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -828,8 +952,11 @@
       <c r="D17" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -838,8 +965,11 @@
       <c r="D18" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
@@ -848,8 +978,11 @@
       <c r="D19" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
@@ -858,8 +991,11 @@
       <c r="D20" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
@@ -868,8 +1004,11 @@
       <c r="D21" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>35</v>
@@ -880,8 +1019,11 @@
       <c r="D22" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
@@ -890,8 +1032,11 @@
       <c r="D23" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -901,7 +1046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -911,7 +1056,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
@@ -925,7 +1070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
@@ -935,7 +1080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
@@ -945,7 +1090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>45</v>
@@ -957,7 +1102,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
@@ -967,7 +1112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
@@ -977,7 +1122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
@@ -987,7 +1132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
@@ -1001,7 +1146,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -1011,7 +1156,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
@@ -1021,7 +1166,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
@@ -1031,7 +1176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="4" t="s">
         <v>55</v>
@@ -1043,7 +1188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
@@ -1053,7 +1198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
@@ -1063,7 +1208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
@@ -1073,7 +1218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="4" t="s">
         <v>60</v>
@@ -1085,7 +1230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
@@ -1095,7 +1240,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
@@ -1105,7 +1250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
@@ -1115,7 +1260,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>65</v>
       </c>
@@ -1129,7 +1274,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
@@ -1139,7 +1284,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
@@ -1149,7 +1294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="4" t="s">
         <v>70</v>
@@ -1161,7 +1306,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
@@ -1171,7 +1316,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
@@ -1181,7 +1326,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
@@ -1191,101 +1336,125 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{95D94DA2-64BF-4E4A-91CE-CA1B52ACA12A}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{67C283BC-D5F3-0A43-9C4F-E3B46F82B6D2}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{E26A744E-94C3-F748-8191-24E5D1C9EFAE}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{98075621-D9A3-9545-BC24-6A6118C2179B}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{831E55ED-BA99-9B41-9438-B4FC6498FFB6}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{D196355F-497F-604E-866D-5036137DE7F7}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{8178CEE4-DDFC-0048-9B5F-9A24DDC7C5E5}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{4E181874-258A-8B43-A7A9-18EE82A13A51}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{9688184B-0637-0B48-91B4-DD46EB7FD4F6}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{367150BF-9145-224F-94B8-B4643E3EEBD7}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{7964E4B8-A1CE-C246-B207-8A95F878883A}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{0E43DB01-108E-BA41-A92D-0A1E1954679B}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{2DB3B9D7-16B4-6A43-B892-DE6961C1C6B2}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{70BC2F1B-C502-1348-BC04-066FFCA385A0}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{245F6CA2-BCB6-8043-A590-E59D608A56A0}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{47CDC467-B9E4-9245-AA08-AF2DBEBD568C}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{C2179527-53EE-054F-BFFB-A8CFF587E7C7}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{0D495A38-0A4B-414F-A8B5-7F3B435AC3E5}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{C3E931A2-8552-D349-B27F-3890DEA920B8}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{6CFB5841-DDF4-B74E-AF7C-D8D47AFF2854}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{80A4DCDB-361E-0842-9FE5-419929A90A5C}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{09F7BD60-F6BA-7E45-B69F-E487B71C23E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>